<commit_message>
Bug fixes and improvements
</commit_message>
<xml_diff>
--- a/Тест-кейси Мірзоян 6.1211-пзс.xlsx
+++ b/Тест-кейси Мірзоян 6.1211-пзс.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wande\OneDrive\Рабочий стол\Практика\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\QA Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -670,125 +670,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -817,6 +724,99 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1100,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,13 +1136,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24">
+      <c r="B3" s="61">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="64" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1151,444 +1151,444 @@
       <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="51" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="14"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="28"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="14"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="28"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="14"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="28"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="65"/>
       <c r="E8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="53"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="20">
+      <c r="B9" s="58">
         <v>2</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="54" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="14"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="35"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="37">
+      <c r="B13" s="43">
         <v>3</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="48" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="36" t="s">
+      <c r="B14" s="45"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="37">
+      <c r="B15" s="43">
         <v>4</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="47" t="s">
+      <c r="G15" s="35" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="48"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="22"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="15"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="48"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="22"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="15"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="48"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="22"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="15"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="48"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="46" t="s">
+      <c r="B20" s="44"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="48"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="15"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="48"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="22"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="46" t="s">
+      <c r="B22" s="44"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="48"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="42"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="36" t="s">
+      <c r="B23" s="45"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="44" t="s">
+      <c r="F23" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="48"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="37">
+      <c r="B24" s="43">
         <v>5</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="50" t="s">
+      <c r="E24" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="35" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="22"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="15"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="48"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="15"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="48"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="22"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="15"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="48"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="22"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="15"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="48"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="22"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="46" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="48"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="22"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="48"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="22"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="46" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="48"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="42"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="36" t="s">
+      <c r="B32" s="45"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="44" t="s">
+      <c r="F32" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="48"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="2:7" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="57">
+      <c r="B33" s="26">
         <v>6</v>
       </c>
-      <c r="C33" s="53" t="s">
+      <c r="C33" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="59" t="s">
+      <c r="F33" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G33" s="60" t="s">
+      <c r="G33" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="65">
+      <c r="B34" s="34">
         <v>7</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E34" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="62"/>
-      <c r="G34" s="63" t="s">
+      <c r="F34" s="31"/>
+      <c r="G34" s="32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C35" s="54"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C36" s="54"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C37" s="54"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C38" s="54"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C39" s="54"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C40" s="54"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C41" s="54"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
@@ -1597,6 +1597,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
     <mergeCell ref="G24:G32"/>
     <mergeCell ref="D24:D32"/>
     <mergeCell ref="C24:C32"/>
@@ -1609,14 +1617,6 @@
     <mergeCell ref="C15:C23"/>
     <mergeCell ref="B15:B23"/>
     <mergeCell ref="G15:G23"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>